<commit_message>
Menambahkan file dan folder baru
</commit_message>
<xml_diff>
--- a/storage/app/templates/Format .xlsx
+++ b/storage/app/templates/Format .xlsx
@@ -768,6 +768,75 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -793,75 +862,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1563,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="62" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="62" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -1596,23 +1596,23 @@
   <sheetData>
     <row r="1" spans="1:29" ht="25.5" customHeight="1"/>
     <row r="4" spans="1:29" ht="18.75" customHeight="1">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="110"/>
-      <c r="N4" s="110"/>
-      <c r="O4" s="110"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -1660,14 +1660,14 @@
       <c r="AC5" s="3"/>
     </row>
     <row r="6" spans="1:29" s="7" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
@@ -1681,14 +1681,14 @@
       </c>
     </row>
     <row r="7" spans="1:29" s="10" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="9"/>
@@ -1702,14 +1702,14 @@
       </c>
     </row>
     <row r="8" spans="1:29" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
@@ -1717,14 +1717,14 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:29" s="7" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
@@ -1845,25 +1845,25 @@
       <c r="A22" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="108" t="s">
+      <c r="E22" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="108"/>
-      <c r="G22" s="108"/>
-      <c r="H22" s="108"/>
-      <c r="I22" s="108"/>
-      <c r="J22" s="109"/>
+      <c r="F22" s="84"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="84"/>
+      <c r="I22" s="84"/>
+      <c r="J22" s="90"/>
       <c r="L22" s="22"/>
       <c r="O22" s="23"/>
     </row>
     <row r="23" spans="1:16" s="7" customFormat="1" ht="60" customHeight="1">
       <c r="A23" s="20"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="108"/>
-      <c r="J23" s="109"/>
+      <c r="E23" s="84"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="84"/>
+      <c r="H23" s="84"/>
+      <c r="I23" s="84"/>
+      <c r="J23" s="90"/>
       <c r="L23" s="20"/>
       <c r="O23" s="21"/>
     </row>
@@ -1895,26 +1895,26 @@
       <c r="A29" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="103" t="s">
+      <c r="B29" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="104"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="104"/>
-      <c r="G29" s="105"/>
-      <c r="H29" s="103" t="s">
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="105"/>
-      <c r="J29" s="106" t="s">
+      <c r="I29" s="87"/>
+      <c r="J29" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="K29" s="107"/>
-      <c r="L29" s="103" t="s">
+      <c r="K29" s="89"/>
+      <c r="L29" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="105"/>
+      <c r="M29" s="87"/>
       <c r="N29" s="27" t="s">
         <v>21</v>
       </c>
@@ -1926,28 +1926,28 @@
       <c r="A30" s="32">
         <v>5</v>
       </c>
-      <c r="B30" s="91" t="s">
+      <c r="B30" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="92"/>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="92"/>
-      <c r="G30" s="93"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="93"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="94"/>
       <c r="H30" s="33">
         <v>10</v>
       </c>
       <c r="I30" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="J30" s="94">
+      <c r="J30" s="95">
         <v>25000</v>
       </c>
-      <c r="K30" s="95"/>
-      <c r="L30" s="96">
+      <c r="K30" s="96"/>
+      <c r="L30" s="97">
         <v>0</v>
       </c>
-      <c r="M30" s="97"/>
+      <c r="M30" s="98"/>
       <c r="N30" s="32" t="s">
         <v>23</v>
       </c>
@@ -1963,16 +1963,16 @@
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
       <c r="H31" s="35"/>
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
       <c r="K31" s="35"/>
-      <c r="L31" s="99" t="s">
+      <c r="L31" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="99"/>
+      <c r="M31" s="100"/>
       <c r="N31" s="36"/>
       <c r="O31" s="37"/>
       <c r="P31" s="31"/>
@@ -2050,16 +2050,16 @@
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
-      <c r="F36" s="100"/>
-      <c r="G36" s="101"/>
+      <c r="F36" s="101"/>
+      <c r="G36" s="102"/>
       <c r="H36" s="44"/>
       <c r="I36" s="43"/>
       <c r="J36" s="43"/>
       <c r="K36" s="43"/>
-      <c r="L36" s="102" t="s">
+      <c r="L36" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="M36" s="102"/>
+      <c r="M36" s="103"/>
       <c r="N36" s="45"/>
       <c r="O36" s="45"/>
     </row>
@@ -2069,8 +2069,8 @@
       <c r="C37" s="43"/>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="102"/>
       <c r="H37" s="44"/>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
@@ -2178,14 +2178,14 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="90"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
       <c r="H43" s="51"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="90"/>
+      <c r="L43" s="91"/>
+      <c r="M43" s="91"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="49"/>
@@ -2204,28 +2204,28 @@
       <c r="I44" s="57"/>
       <c r="J44" s="30"/>
       <c r="K44" s="6"/>
-      <c r="L44" s="82"/>
-      <c r="M44" s="82"/>
+      <c r="L44" s="105"/>
+      <c r="M44" s="105"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="52"/>
     </row>
     <row r="45" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A45" s="83" t="s">
+      <c r="A45" s="106" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="84"/>
-      <c r="C45" s="84"/>
-      <c r="D45" s="84"/>
-      <c r="E45" s="84"/>
-      <c r="F45" s="84"/>
-      <c r="G45" s="84"/>
-      <c r="H45" s="84"/>
-      <c r="I45" s="84"/>
-      <c r="J45" s="85"/>
+      <c r="B45" s="107"/>
+      <c r="C45" s="107"/>
+      <c r="D45" s="107"/>
+      <c r="E45" s="107"/>
+      <c r="F45" s="107"/>
+      <c r="G45" s="107"/>
+      <c r="H45" s="107"/>
+      <c r="I45" s="107"/>
+      <c r="J45" s="108"/>
       <c r="K45" s="7"/>
-      <c r="L45" s="81"/>
-      <c r="M45" s="81"/>
+      <c r="L45" s="104"/>
+      <c r="M45" s="104"/>
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
       <c r="P45" s="52"/>
@@ -2236,14 +2236,14 @@
       <c r="C46" s="60"/>
       <c r="D46" s="60"/>
       <c r="E46" s="60"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="86"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
       <c r="H46" s="61"/>
       <c r="I46" s="60"/>
       <c r="J46" s="62"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="81"/>
-      <c r="M46" s="81"/>
+      <c r="L46" s="104"/>
+      <c r="M46" s="104"/>
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
       <c r="P46" s="52"/>
@@ -2254,14 +2254,14 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
-      <c r="F47" s="81"/>
-      <c r="G47" s="81"/>
+      <c r="F47" s="104"/>
+      <c r="G47" s="104"/>
       <c r="H47" s="63"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="81"/>
-      <c r="M47" s="81"/>
+      <c r="L47" s="104"/>
+      <c r="M47" s="104"/>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
     </row>
@@ -2278,17 +2278,17 @@
       <c r="H48" s="63"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
-      <c r="L48" s="81"/>
-      <c r="M48" s="81"/>
+      <c r="L48" s="104"/>
+      <c r="M48" s="104"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
     </row>
     <row r="49" spans="1:17" s="7" customFormat="1" ht="15.5">
-      <c r="F49" s="81"/>
-      <c r="G49" s="81"/>
+      <c r="F49" s="104"/>
+      <c r="G49" s="104"/>
       <c r="H49" s="63"/>
-      <c r="L49" s="81"/>
-      <c r="M49" s="81"/>
+      <c r="L49" s="104"/>
+      <c r="M49" s="104"/>
       <c r="Q49" s="58"/>
     </row>
     <row r="50" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
@@ -2446,37 +2446,37 @@
       <c r="O57" s="7"/>
     </row>
     <row r="58" spans="1:17" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A58" s="87" t="s">
+      <c r="A58" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="88"/>
-      <c r="C58" s="88"/>
-      <c r="D58" s="88"/>
-      <c r="E58" s="88"/>
-      <c r="F58" s="88"/>
-      <c r="G58" s="88"/>
-      <c r="H58" s="88"/>
-      <c r="I58" s="88"/>
-      <c r="J58" s="88"/>
-      <c r="K58" s="88"/>
-      <c r="L58" s="89"/>
+      <c r="B58" s="111"/>
+      <c r="C58" s="111"/>
+      <c r="D58" s="111"/>
+      <c r="E58" s="111"/>
+      <c r="F58" s="111"/>
+      <c r="G58" s="111"/>
+      <c r="H58" s="111"/>
+      <c r="I58" s="111"/>
+      <c r="J58" s="111"/>
+      <c r="K58" s="111"/>
+      <c r="L58" s="112"/>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
     </row>
     <row r="59" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A59" s="87"/>
-      <c r="B59" s="88"/>
-      <c r="C59" s="88"/>
-      <c r="D59" s="88"/>
-      <c r="E59" s="88"/>
-      <c r="F59" s="88"/>
-      <c r="G59" s="88"/>
-      <c r="H59" s="88"/>
-      <c r="I59" s="88"/>
-      <c r="J59" s="88"/>
-      <c r="K59" s="88"/>
-      <c r="L59" s="89"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="111"/>
+      <c r="C59" s="111"/>
+      <c r="D59" s="111"/>
+      <c r="E59" s="111"/>
+      <c r="F59" s="111"/>
+      <c r="G59" s="111"/>
+      <c r="H59" s="111"/>
+      <c r="I59" s="111"/>
+      <c r="J59" s="111"/>
+      <c r="K59" s="111"/>
+      <c r="L59" s="112"/>
     </row>
     <row r="60" spans="1:17" s="7" customFormat="1" ht="15.5">
       <c r="A60" s="59"/>
@@ -2543,11 +2543,11 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="81" t="s">
+      <c r="M63" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="N63" s="81"/>
-      <c r="O63" s="81"/>
+      <c r="N63" s="104"/>
+      <c r="O63" s="104"/>
       <c r="P63" s="63"/>
     </row>
     <row r="64" spans="1:17" s="7" customFormat="1" ht="15.5">
@@ -2563,37 +2563,17 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="81" t="s">
+      <c r="M64" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="N64" s="81"/>
-      <c r="O64" s="81"/>
+      <c r="N64" s="104"/>
+      <c r="O64" s="104"/>
       <c r="P64" s="63"/>
     </row>
     <row r="67" ht="16.5" customHeight="1"/>
     <row r="68" ht="16.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="E22:J23"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="F37:G37"/>
     <mergeCell ref="M64:O64"/>
     <mergeCell ref="L44:M44"/>
     <mergeCell ref="A45:J45"/>
@@ -2607,6 +2587,26 @@
     <mergeCell ref="L49:M49"/>
     <mergeCell ref="A58:L59"/>
     <mergeCell ref="M63:O63"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="E22:J23"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0" top="0.51181102362204722" bottom="0.23622047244094491" header="0" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="61" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix : Inv & surat jalan export
</commit_message>
<xml_diff>
--- a/storage/app/templates/Format .xlsx
+++ b/storage/app/templates/Format .xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>PT RPN - PUSAT PENELITIAN PERKEBUNAN GULA INDONESIA</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>: …..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. Penawaran: </t>
   </si>
   <si>
     <t>brng</t>
@@ -529,7 +526,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -780,6 +777,81 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -789,109 +861,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1593,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A23" zoomScale="62" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A47" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.5"/>
@@ -1626,23 +1617,23 @@
   <sheetData>
     <row r="1" spans="1:29" ht="25.5" customHeight="1"/>
     <row r="4" spans="1:29" ht="18.75" customHeight="1">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="110"/>
-      <c r="N4" s="110"/>
-      <c r="O4" s="110"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="86"/>
+      <c r="O4" s="86"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -1690,14 +1681,14 @@
       <c r="AC5" s="3"/>
     </row>
     <row r="6" spans="1:29" s="7" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="5"/>
@@ -1711,14 +1702,14 @@
       </c>
     </row>
     <row r="7" spans="1:29" s="10" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A7" s="112" t="s">
+      <c r="A7" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="112"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="9"/>
@@ -1732,14 +1723,14 @@
       </c>
     </row>
     <row r="8" spans="1:29" s="7" customFormat="1" ht="18" customHeight="1">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="108"/>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
@@ -1747,14 +1738,14 @@
       <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:29" s="7" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="89"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
@@ -1875,25 +1866,25 @@
       <c r="A22" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="108" t="s">
+      <c r="E22" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="108"/>
-      <c r="G22" s="108"/>
-      <c r="H22" s="108"/>
-      <c r="I22" s="108"/>
-      <c r="J22" s="109"/>
+      <c r="F22" s="89"/>
+      <c r="G22" s="89"/>
+      <c r="H22" s="89"/>
+      <c r="I22" s="89"/>
+      <c r="J22" s="95"/>
       <c r="L22" s="22"/>
       <c r="O22" s="23"/>
     </row>
     <row r="23" spans="1:16" s="7" customFormat="1" ht="60" customHeight="1">
       <c r="A23" s="20"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="108"/>
-      <c r="J23" s="109"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="95"/>
       <c r="L23" s="20"/>
       <c r="O23" s="21"/>
     </row>
@@ -1925,26 +1916,26 @@
       <c r="A29" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="103" t="s">
+      <c r="B29" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="104"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="104"/>
-      <c r="G29" s="105"/>
-      <c r="H29" s="103" t="s">
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="105"/>
-      <c r="J29" s="106" t="s">
+      <c r="I29" s="92"/>
+      <c r="J29" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="K29" s="107"/>
-      <c r="L29" s="103" t="s">
+      <c r="K29" s="94"/>
+      <c r="L29" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="105"/>
+      <c r="M29" s="92"/>
       <c r="N29" s="27" t="s">
         <v>21</v>
       </c>
@@ -1956,28 +1947,28 @@
       <c r="A30" s="32">
         <v>5</v>
       </c>
-      <c r="B30" s="91" t="s">
+      <c r="B30" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="92"/>
-      <c r="D30" s="92"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="92"/>
-      <c r="G30" s="93"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="99"/>
       <c r="H30" s="33">
         <v>10</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="J30" s="94">
+        <v>48</v>
+      </c>
+      <c r="J30" s="100">
         <v>25000</v>
       </c>
-      <c r="K30" s="95"/>
-      <c r="L30" s="96">
+      <c r="K30" s="101"/>
+      <c r="L30" s="102">
         <v>0</v>
       </c>
-      <c r="M30" s="97"/>
+      <c r="M30" s="103"/>
       <c r="N30" s="32" t="s">
         <v>23</v>
       </c>
@@ -1993,16 +1984,16 @@
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
       <c r="E31" s="35"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="98"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
       <c r="H31" s="35"/>
       <c r="I31" s="35"/>
       <c r="J31" s="35"/>
       <c r="K31" s="35"/>
-      <c r="L31" s="99" t="s">
+      <c r="L31" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="M31" s="99"/>
+      <c r="M31" s="105"/>
       <c r="N31" s="36"/>
       <c r="O31" s="37"/>
       <c r="P31" s="31"/>
@@ -2025,7 +2016,7 @@
       <c r="M32" s="41"/>
       <c r="N32" s="41"/>
       <c r="O32" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:17" s="6" customFormat="1" ht="24" customHeight="1">
@@ -2082,16 +2073,16 @@
       <c r="C36" s="43"/>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
-      <c r="F36" s="100"/>
-      <c r="G36" s="101"/>
+      <c r="F36" s="106"/>
+      <c r="G36" s="107"/>
       <c r="H36" s="44"/>
       <c r="I36" s="43"/>
       <c r="J36" s="43"/>
       <c r="K36" s="43"/>
-      <c r="L36" s="102" t="s">
+      <c r="L36" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="M36" s="102"/>
+      <c r="M36" s="108"/>
       <c r="N36" s="45"/>
       <c r="O36" s="45"/>
     </row>
@@ -2101,8 +2092,8 @@
       <c r="C37" s="43"/>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
+      <c r="F37" s="107"/>
+      <c r="G37" s="107"/>
       <c r="H37" s="44"/>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
@@ -2210,14 +2201,14 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="90"/>
-      <c r="G43" s="90"/>
+      <c r="F43" s="96"/>
+      <c r="G43" s="96"/>
       <c r="H43" s="51"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="90"/>
-      <c r="M43" s="90"/>
+      <c r="L43" s="96"/>
+      <c r="M43" s="96"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="49"/>
@@ -2236,34 +2227,32 @@
       <c r="I44" s="57"/>
       <c r="J44" s="30"/>
       <c r="K44" s="6"/>
-      <c r="L44" s="85"/>
-      <c r="M44" s="85"/>
+      <c r="L44" s="110"/>
+      <c r="M44" s="110"/>
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="52"/>
     </row>
     <row r="45" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A45" s="86" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="120"/>
-      <c r="C45" s="120"/>
-      <c r="D45" s="120"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="120"/>
-      <c r="G45" s="120"/>
-      <c r="H45" s="120"/>
-      <c r="I45" s="120"/>
-      <c r="J45" s="87"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="112"/>
+      <c r="E45" s="112"/>
+      <c r="F45" s="112"/>
+      <c r="G45" s="112"/>
+      <c r="H45" s="112"/>
+      <c r="I45" s="112"/>
+      <c r="J45" s="113"/>
       <c r="K45" s="7"/>
-      <c r="L45" s="84"/>
-      <c r="M45" s="84"/>
+      <c r="L45" s="109"/>
+      <c r="M45" s="109"/>
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
       <c r="P45" s="52"/>
     </row>
     <row r="46" spans="1:17" ht="18.75" customHeight="1">
-      <c r="A46" s="86"/>
+      <c r="A46" s="114"/>
       <c r="B46" s="115"/>
       <c r="C46" s="115"/>
       <c r="D46" s="115"/>
@@ -2274,65 +2263,71 @@
       <c r="I46" s="115"/>
       <c r="J46" s="116"/>
       <c r="K46" s="7"/>
-      <c r="L46" s="84"/>
-      <c r="M46" s="84"/>
+      <c r="L46" s="109"/>
+      <c r="M46" s="109"/>
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
       <c r="P46" s="52"/>
     </row>
     <row r="47" spans="1:17" ht="15.5">
-      <c r="A47" s="117"/>
-      <c r="B47" s="118"/>
-      <c r="C47" s="118"/>
-      <c r="D47" s="118"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
-      <c r="G47" s="118"/>
-      <c r="H47" s="118"/>
-      <c r="I47" s="118"/>
-      <c r="J47" s="119"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="109"/>
+      <c r="G47" s="109"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
       <c r="K47" s="7"/>
-      <c r="L47" s="84"/>
-      <c r="M47" s="84"/>
+      <c r="L47" s="109"/>
+      <c r="M47" s="109"/>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
     </row>
     <row r="48" spans="1:17" s="6" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="84"/>
-      <c r="G48" s="84"/>
+      <c r="A48" s="63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="63"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
       <c r="H48" s="62"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
-      <c r="L48" s="84"/>
-      <c r="M48" s="84"/>
+      <c r="L48" s="109"/>
+      <c r="M48" s="109"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
-      <c r="Q48" s="114"/>
+      <c r="Q48" s="85"/>
     </row>
     <row r="49" spans="1:17" s="7" customFormat="1" ht="15.5">
-      <c r="A49" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
+      <c r="F49" s="109"/>
+      <c r="G49" s="109"/>
       <c r="H49" s="62"/>
-      <c r="L49" s="84"/>
-      <c r="M49" s="84"/>
-      <c r="Q49" s="113"/>
+      <c r="L49" s="109"/>
+      <c r="M49" s="109"/>
+      <c r="Q49" s="84"/>
     </row>
     <row r="50" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="F50" s="84"/>
-      <c r="G50" s="84"/>
-      <c r="H50" s="62"/>
+      <c r="A50" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="65"/>
+      <c r="C50" s="65"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" s="65"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="65"/>
+      <c r="J50" s="66"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
@@ -2340,20 +2335,20 @@
       <c r="O50" s="6"/>
     </row>
     <row r="51" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A51" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="65"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="65"/>
-      <c r="E51" s="65"/>
-      <c r="F51" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="G51" s="65"/>
-      <c r="H51" s="65"/>
-      <c r="I51" s="65"/>
-      <c r="J51" s="66"/>
+      <c r="A51" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="68"/>
+      <c r="C51" s="68"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="68" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" s="68"/>
+      <c r="H51" s="68"/>
+      <c r="I51" s="68"/>
+      <c r="J51" s="69"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
@@ -2362,14 +2357,14 @@
     </row>
     <row r="52" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A52" s="67" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B52" s="68"/>
       <c r="C52" s="68"/>
       <c r="D52" s="68"/>
       <c r="E52" s="68"/>
-      <c r="F52" s="68" t="s">
-        <v>37</v>
+      <c r="F52" s="70" t="s">
+        <v>39</v>
       </c>
       <c r="G52" s="68"/>
       <c r="H52" s="68"/>
@@ -2383,14 +2378,14 @@
     </row>
     <row r="53" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A53" s="67" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B53" s="68"/>
       <c r="C53" s="68"/>
       <c r="D53" s="68"/>
       <c r="E53" s="68"/>
-      <c r="F53" s="70" t="s">
-        <v>39</v>
+      <c r="F53" s="68" t="s">
+        <v>41</v>
       </c>
       <c r="G53" s="68"/>
       <c r="H53" s="68"/>
@@ -2403,37 +2398,33 @@
       <c r="O53" s="6"/>
     </row>
     <row r="54" spans="1:17" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A54" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="B54" s="68"/>
-      <c r="C54" s="68"/>
-      <c r="D54" s="68"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="69"/>
+      <c r="A54" s="71"/>
+      <c r="B54" s="72"/>
+      <c r="C54" s="72"/>
+      <c r="D54" s="72"/>
+      <c r="E54" s="72"/>
+      <c r="F54" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="G54" s="72"/>
+      <c r="H54" s="72"/>
+      <c r="I54" s="72"/>
+      <c r="J54" s="73"/>
       <c r="M54" s="7"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
     </row>
     <row r="55" spans="1:17" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A55" s="71"/>
-      <c r="B55" s="72"/>
-      <c r="C55" s="72"/>
-      <c r="D55" s="72"/>
-      <c r="E55" s="72"/>
-      <c r="F55" s="72" t="s">
-        <v>42</v>
-      </c>
-      <c r="G55" s="72"/>
-      <c r="H55" s="72"/>
-      <c r="I55" s="72"/>
-      <c r="J55" s="73"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
       <c r="K55" s="80"/>
       <c r="L55" s="80"/>
       <c r="M55" s="7"/>
@@ -2441,104 +2432,104 @@
       <c r="O55" s="7"/>
     </row>
     <row r="56" spans="1:17" s="6" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
+      <c r="A56" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B56" s="58"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="58"/>
+      <c r="F56" s="58"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
+      <c r="J56" s="58"/>
+      <c r="K56" s="58"/>
+      <c r="L56" s="75"/>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
       <c r="O56" s="7"/>
     </row>
     <row r="57" spans="1:17" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A57" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" s="58"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="58"/>
-      <c r="L57" s="75"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="21"/>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
       <c r="O57" s="7"/>
     </row>
     <row r="58" spans="1:17" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A58" s="20"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="21"/>
+      <c r="A58" s="117" t="s">
+        <v>44</v>
+      </c>
+      <c r="B58" s="118"/>
+      <c r="C58" s="118"/>
+      <c r="D58" s="118"/>
+      <c r="E58" s="118"/>
+      <c r="F58" s="118"/>
+      <c r="G58" s="118"/>
+      <c r="H58" s="118"/>
+      <c r="I58" s="118"/>
+      <c r="J58" s="118"/>
+      <c r="K58" s="118"/>
+      <c r="L58" s="119"/>
       <c r="M58" s="7"/>
       <c r="N58" s="7"/>
       <c r="O58" s="7"/>
     </row>
     <row r="59" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A59" s="88" t="s">
-        <v>44</v>
-      </c>
-      <c r="B59" s="121"/>
-      <c r="C59" s="121"/>
-      <c r="D59" s="121"/>
-      <c r="E59" s="121"/>
-      <c r="F59" s="121"/>
-      <c r="G59" s="121"/>
-      <c r="H59" s="121"/>
-      <c r="I59" s="121"/>
-      <c r="J59" s="121"/>
-      <c r="K59" s="121"/>
-      <c r="L59" s="89"/>
+      <c r="A59" s="81"/>
+      <c r="B59" s="82"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="82"/>
+      <c r="E59" s="82"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
+      <c r="H59" s="82"/>
+      <c r="I59" s="82"/>
+      <c r="J59" s="82"/>
+      <c r="K59" s="82"/>
+      <c r="L59" s="83"/>
     </row>
     <row r="60" spans="1:17" s="7" customFormat="1" ht="15.5">
-      <c r="A60" s="81"/>
-      <c r="B60" s="82"/>
-      <c r="C60" s="82"/>
-      <c r="D60" s="82"/>
-      <c r="E60" s="82"/>
-      <c r="F60" s="82"/>
-      <c r="G60" s="82"/>
-      <c r="H60" s="82"/>
-      <c r="I60" s="82"/>
-      <c r="J60" s="82"/>
-      <c r="K60" s="82"/>
-      <c r="L60" s="83"/>
+      <c r="A60" s="59"/>
+      <c r="B60" s="60"/>
+      <c r="C60" s="60"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="60"/>
+      <c r="F60" s="60"/>
+      <c r="G60" s="60"/>
+      <c r="H60" s="60"/>
+      <c r="I60" s="60"/>
+      <c r="J60" s="60"/>
+      <c r="K60" s="60"/>
+      <c r="L60" s="61"/>
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
     </row>
     <row r="61" spans="1:17" s="7" customFormat="1" ht="15" customHeight="1">
-      <c r="A61" s="59"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="60"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="60"/>
-      <c r="F61" s="60"/>
-      <c r="G61" s="60"/>
-      <c r="H61" s="60"/>
-      <c r="I61" s="60"/>
-      <c r="J61" s="60"/>
-      <c r="K61" s="60"/>
-      <c r="L61" s="61"/>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
@@ -2574,11 +2565,11 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="84" t="s">
+      <c r="M63" s="109" t="s">
         <v>45</v>
       </c>
-      <c r="N63" s="84"/>
-      <c r="O63" s="84"/>
+      <c r="N63" s="109"/>
+      <c r="O63" s="109"/>
       <c r="P63" s="62"/>
     </row>
     <row r="64" spans="1:17" s="7" customFormat="1" ht="15.5">
@@ -2594,27 +2585,29 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="84" t="s">
+      <c r="M64" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="N64" s="84"/>
-      <c r="O64" s="84"/>
+      <c r="N64" s="109"/>
+      <c r="O64" s="109"/>
       <c r="P64" s="62"/>
     </row>
     <row r="67" ht="16.5" customHeight="1"/>
     <row r="68" ht="16.5" customHeight="1"/>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="E22:J23"/>
+  <mergeCells count="32">
+    <mergeCell ref="M64:O64"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="M63:O63"/>
+    <mergeCell ref="A45:J46"/>
+    <mergeCell ref="A58:L58"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="L43:M43"/>
     <mergeCell ref="B30:G30"/>
@@ -2625,19 +2618,16 @@
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="L36:M36"/>
     <mergeCell ref="F37:G37"/>
-    <mergeCell ref="M64:O64"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="M63:O63"/>
-    <mergeCell ref="A46:J47"/>
-    <mergeCell ref="A59:L59"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="E22:J23"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0" top="0.51181102362204722" bottom="0.23622047244094491" header="0" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="61" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>